<commit_message>
hoàn thành BT tuần này
</commit_message>
<xml_diff>
--- a/Document/Design/SDD_Login.xlsx
+++ b/Document/Design/SDD_Login.xlsx
@@ -17,15 +17,166 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Contents!$A$1:$E$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Cover!$A$1:$D$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'Screen Detail'!$B$2:$BE$65</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Screen Detail'!$B$2:$BE$73</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Signature!$A$1:$F$24</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Trinh Anh Linh</author>
+  </authors>
+  <commentList>
+    <comment ref="W13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LinhTA:
+pnlError : hide</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LinhTA:
+txtUsername</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LinhTA:
+txtPassword</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LinhTA:
+cboLanguage</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LinhTA:
+linkReturnToSiteHomePage</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">LinhTA:
+btnLogin
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
   <si>
     <t>&lt;Project Name&gt;</t>
   </si>
@@ -132,9 +283,6 @@
     <t>4. Events</t>
   </si>
   <si>
-    <t>&lt;This place you can put pictures or some thing else to describe your screen and how to lay out its items&gt;</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -238,13 +386,106 @@
   </si>
   <si>
     <t>10/15/2011</t>
+  </si>
+  <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>DB Table Name</t>
+  </si>
+  <si>
+    <t>DB Column Name</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>Trở lại trang chủ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">So sánh dữ liệu trên txtUsername và txtPassword với CSDL, nếu đúng thì vào trang quản lý, sai thì hiện pnlError báo lỗi đăng nhập </t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Tên đăng nhập dành cho quản lý website</t>
+  </si>
+  <si>
+    <t>Mật khẩu đăng nhập dành cho quản lý website</t>
+  </si>
+  <si>
+    <t>Lưu đường dẫn đến thư viện ngôn ngữ hỗ trợ cho website</t>
+  </si>
+  <si>
+    <t>LinkLanguage</t>
+  </si>
+  <si>
+    <t>Lưu tên ngôn ngữ</t>
+  </si>
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
+  </si>
+  <si>
+    <t>LanguageName</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>CMS Login</t>
+  </si>
+  <si>
+    <t>&lt;Icon&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Error&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Guide use&gt;</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>Return to site Home Page</t>
+  </si>
+  <si>
+    <t>&lt;Picture&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="16">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,8 +587,57 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Rounded MT Bold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,8 +656,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -717,11 +1019,176 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -781,67 +1248,171 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1210,14 +1781,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="33">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="1" t="s">
@@ -1437,12 +2008,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="33">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="5" spans="2:5" ht="15.75">
       <c r="B5" s="21" t="s">
@@ -1504,11 +2075,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="33">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="22"/>
@@ -1690,147 +2261,150 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:BE54"/>
+  <dimension ref="B2:BE64"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BD10" sqref="BD10"/>
+      <pane ySplit="5" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AM16" sqref="AM16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="4" width="3.125" style="32" customWidth="1"/>
-    <col min="5" max="60" width="3.625" style="32" customWidth="1"/>
+    <col min="5" max="5" width="9.75" style="32" customWidth="1"/>
+    <col min="6" max="17" width="3.625" style="32" customWidth="1"/>
+    <col min="18" max="18" width="9.25" style="32" customWidth="1"/>
+    <col min="19" max="60" width="3.625" style="32" customWidth="1"/>
     <col min="61" max="16384" width="9" style="32"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:57">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="52" t="s">
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="52"/>
-      <c r="Z2" s="52"/>
-      <c r="AA2" s="52"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="52"/>
-      <c r="AD2" s="52"/>
-      <c r="AE2" s="52"/>
-      <c r="AF2" s="52"/>
-      <c r="AG2" s="52"/>
-      <c r="AH2" s="52"/>
-      <c r="AI2" s="52"/>
-      <c r="AJ2" s="52"/>
-      <c r="AK2" s="52"/>
-      <c r="AL2" s="52"/>
-      <c r="AM2" s="52"/>
-      <c r="AN2" s="52"/>
-      <c r="AO2" s="52"/>
-      <c r="AP2" s="52"/>
-      <c r="AQ2" s="54" t="s">
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+      <c r="X2" s="57"/>
+      <c r="Y2" s="57"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
+      <c r="AF2" s="57"/>
+      <c r="AG2" s="57"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
-      <c r="AW2" s="54"/>
-      <c r="AX2" s="54" t="s">
+      <c r="AR2" s="52"/>
+      <c r="AS2" s="52"/>
+      <c r="AT2" s="52"/>
+      <c r="AU2" s="52"/>
+      <c r="AV2" s="52"/>
+      <c r="AW2" s="52"/>
+      <c r="AX2" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="AY2" s="54"/>
-      <c r="AZ2" s="54"/>
-      <c r="BA2" s="54"/>
-      <c r="BB2" s="54"/>
-      <c r="BC2" s="54"/>
-      <c r="BD2" s="54"/>
-      <c r="BE2" s="54"/>
+      <c r="AY2" s="52"/>
+      <c r="AZ2" s="52"/>
+      <c r="BA2" s="52"/>
+      <c r="BB2" s="52"/>
+      <c r="BC2" s="52"/>
+      <c r="BD2" s="52"/>
+      <c r="BE2" s="52"/>
     </row>
     <row r="3" spans="2:57">
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52"/>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="52"/>
-      <c r="Z3" s="52"/>
-      <c r="AA3" s="52"/>
-      <c r="AB3" s="52"/>
-      <c r="AC3" s="52"/>
-      <c r="AD3" s="52"/>
-      <c r="AE3" s="52"/>
-      <c r="AF3" s="52"/>
-      <c r="AG3" s="52"/>
-      <c r="AH3" s="52"/>
-      <c r="AI3" s="52"/>
-      <c r="AJ3" s="52"/>
-      <c r="AK3" s="52"/>
-      <c r="AL3" s="52"/>
-      <c r="AM3" s="52"/>
-      <c r="AN3" s="52"/>
-      <c r="AO3" s="52"/>
-      <c r="AP3" s="52"/>
-      <c r="AQ3" s="55" t="s">
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="57"/>
+      <c r="X3" s="57"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="57"/>
+      <c r="AA3" s="57"/>
+      <c r="AB3" s="57"/>
+      <c r="AC3" s="57"/>
+      <c r="AD3" s="57"/>
+      <c r="AE3" s="57"/>
+      <c r="AF3" s="57"/>
+      <c r="AG3" s="57"/>
+      <c r="AH3" s="57"/>
+      <c r="AI3" s="57"/>
+      <c r="AJ3" s="57"/>
+      <c r="AK3" s="57"/>
+      <c r="AL3" s="57"/>
+      <c r="AM3" s="57"/>
+      <c r="AN3" s="57"/>
+      <c r="AO3" s="57"/>
+      <c r="AP3" s="57"/>
+      <c r="AQ3" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR3" s="54"/>
+      <c r="AS3" s="54"/>
+      <c r="AT3" s="54"/>
+      <c r="AU3" s="54"/>
+      <c r="AV3" s="54"/>
+      <c r="AW3" s="54"/>
+      <c r="AX3" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="AR3" s="55"/>
-      <c r="AS3" s="55"/>
-      <c r="AT3" s="55"/>
-      <c r="AU3" s="55"/>
-      <c r="AV3" s="55"/>
-      <c r="AW3" s="55"/>
-      <c r="AX3" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="AY3" s="55"/>
-      <c r="AZ3" s="55"/>
-      <c r="BA3" s="55"/>
-      <c r="BB3" s="55"/>
-      <c r="BC3" s="55"/>
-      <c r="BD3" s="55"/>
-      <c r="BE3" s="55"/>
+      <c r="AY3" s="54"/>
+      <c r="AZ3" s="54"/>
+      <c r="BA3" s="54"/>
+      <c r="BB3" s="54"/>
+      <c r="BC3" s="54"/>
+      <c r="BD3" s="54"/>
+      <c r="BE3" s="54"/>
     </row>
     <row r="4" spans="2:57">
       <c r="B4" s="31" t="s">
@@ -1857,7 +2431,7 @@
       <c r="S4" s="31"/>
       <c r="T4" s="31"/>
       <c r="U4" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V4" s="53"/>
       <c r="W4" s="53"/>
@@ -1886,7 +2460,7 @@
       <c r="AR4" s="31"/>
       <c r="AS4" s="31"/>
       <c r="AT4" s="53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU4" s="53"/>
       <c r="AV4" s="53"/>
@@ -1898,7 +2472,7 @@
       <c r="AZ4" s="31"/>
       <c r="BA4" s="31"/>
       <c r="BB4" s="53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BC4" s="53"/>
       <c r="BD4" s="53"/>
@@ -1956,7 +2530,7 @@
       <c r="AR5" s="31"/>
       <c r="AS5" s="31"/>
       <c r="AT5" s="53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU5" s="53"/>
       <c r="AV5" s="53"/>
@@ -1968,7 +2542,7 @@
       <c r="AZ5" s="31"/>
       <c r="BA5" s="31"/>
       <c r="BB5" s="53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BC5" s="53"/>
       <c r="BD5" s="53"/>
@@ -1979,562 +2553,2226 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:57">
-      <c r="C9" s="34" t="s">
+    <row r="9" spans="2:57" ht="14.25">
+      <c r="C9" s="34"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="66"/>
+      <c r="T9" s="66"/>
+      <c r="U9" s="66"/>
+      <c r="V9" s="66"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="66"/>
+      <c r="Y9" s="66"/>
+      <c r="Z9" s="66"/>
+      <c r="AA9" s="66"/>
+      <c r="AB9" s="66"/>
+      <c r="AC9" s="66"/>
+      <c r="AD9" s="66"/>
+      <c r="AE9" s="66"/>
+      <c r="AF9" s="66"/>
+      <c r="AG9" s="66"/>
+      <c r="AH9" s="66"/>
+      <c r="AI9" s="66"/>
+      <c r="AJ9" s="66"/>
+      <c r="AK9" s="66"/>
+      <c r="AL9" s="66"/>
+      <c r="AM9" s="66"/>
+      <c r="AN9" s="66"/>
+      <c r="AO9" s="66"/>
+      <c r="AP9" s="66"/>
+      <c r="AQ9" s="66"/>
+      <c r="AR9" s="67"/>
+    </row>
+    <row r="10" spans="2:57" ht="14.25">
+      <c r="G10" s="68"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="64"/>
+      <c r="P10" s="64"/>
+      <c r="Q10" s="64"/>
+      <c r="R10" s="64"/>
+      <c r="S10" s="64"/>
+      <c r="T10" s="64"/>
+      <c r="U10" s="64"/>
+      <c r="V10" s="64"/>
+      <c r="W10" s="64"/>
+      <c r="X10" s="64"/>
+      <c r="Y10" s="64"/>
+      <c r="Z10" s="64"/>
+      <c r="AA10" s="64"/>
+      <c r="AB10" s="64"/>
+      <c r="AC10" s="64"/>
+      <c r="AD10" s="64"/>
+      <c r="AE10" s="64"/>
+      <c r="AF10" s="64"/>
+      <c r="AG10" s="64"/>
+      <c r="AH10" s="64"/>
+      <c r="AI10" s="64"/>
+      <c r="AJ10" s="64"/>
+      <c r="AK10" s="64"/>
+      <c r="AL10" s="64"/>
+      <c r="AM10" s="64"/>
+      <c r="AN10" s="64"/>
+      <c r="AO10" s="64"/>
+      <c r="AP10" s="64"/>
+      <c r="AQ10" s="64"/>
+      <c r="AR10" s="69"/>
+    </row>
+    <row r="11" spans="2:57" ht="14.25">
+      <c r="G11" s="68"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="64"/>
+      <c r="R11" s="77" t="s">
+        <v>92</v>
+      </c>
+      <c r="S11" s="78"/>
+      <c r="T11" s="78"/>
+      <c r="U11" s="78"/>
+      <c r="V11" s="78"/>
+      <c r="W11" s="78"/>
+      <c r="X11" s="78"/>
+      <c r="Y11" s="78"/>
+      <c r="Z11" s="78"/>
+      <c r="AA11" s="66"/>
+      <c r="AB11" s="66"/>
+      <c r="AC11" s="66"/>
+      <c r="AD11" s="66"/>
+      <c r="AE11" s="66"/>
+      <c r="AF11" s="66"/>
+      <c r="AG11" s="66"/>
+      <c r="AH11" s="67"/>
+      <c r="AI11" s="64"/>
+      <c r="AJ11" s="64"/>
+      <c r="AK11" s="64"/>
+      <c r="AL11" s="64"/>
+      <c r="AM11" s="64"/>
+      <c r="AN11" s="64"/>
+      <c r="AO11" s="64"/>
+      <c r="AP11" s="64"/>
+      <c r="AQ11" s="64"/>
+      <c r="AR11" s="69"/>
+    </row>
+    <row r="12" spans="2:57" ht="14.25">
+      <c r="G12" s="68"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="64"/>
+      <c r="R12" s="79"/>
+      <c r="S12" s="80"/>
+      <c r="T12" s="80"/>
+      <c r="U12" s="80"/>
+      <c r="V12" s="80"/>
+      <c r="W12" s="80"/>
+      <c r="X12" s="80"/>
+      <c r="Y12" s="80"/>
+      <c r="Z12" s="80"/>
+      <c r="AA12" s="74"/>
+      <c r="AB12" s="74"/>
+      <c r="AC12" s="74"/>
+      <c r="AD12" s="74"/>
+      <c r="AE12" s="74"/>
+      <c r="AF12" s="74"/>
+      <c r="AG12" s="74"/>
+      <c r="AH12" s="75"/>
+      <c r="AI12" s="64"/>
+      <c r="AJ12" s="64"/>
+      <c r="AK12" s="64"/>
+      <c r="AL12" s="64"/>
+      <c r="AM12" s="64"/>
+      <c r="AN12" s="64"/>
+      <c r="AO12" s="64"/>
+      <c r="AP12" s="64"/>
+      <c r="AQ12" s="64"/>
+      <c r="AR12" s="69"/>
+    </row>
+    <row r="13" spans="2:57" ht="14.25">
+      <c r="G13" s="68"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="63"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="69"/>
+      <c r="R13" s="64"/>
+      <c r="S13" s="64"/>
+      <c r="T13" s="100" t="s">
+        <v>93</v>
+      </c>
+      <c r="U13" s="101"/>
+      <c r="V13" s="64"/>
+      <c r="W13" s="100" t="s">
+        <v>94</v>
+      </c>
+      <c r="X13" s="100"/>
+      <c r="Y13" s="100"/>
+      <c r="Z13" s="100"/>
+      <c r="AA13" s="100"/>
+      <c r="AB13" s="100"/>
+      <c r="AC13" s="100"/>
+      <c r="AD13" s="100"/>
+      <c r="AE13" s="100"/>
+      <c r="AF13" s="100"/>
+      <c r="AG13" s="100"/>
+      <c r="AH13" s="101"/>
+      <c r="AI13" s="64"/>
+      <c r="AJ13" s="64"/>
+      <c r="AK13" s="64"/>
+      <c r="AL13" s="64"/>
+      <c r="AM13" s="64"/>
+      <c r="AN13" s="64"/>
+      <c r="AO13" s="64"/>
+      <c r="AP13" s="64"/>
+      <c r="AQ13" s="64"/>
+      <c r="AR13" s="69"/>
+    </row>
+    <row r="14" spans="2:57" ht="14.25">
+      <c r="G14" s="68"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="69"/>
+      <c r="R14" s="64"/>
+      <c r="S14" s="64"/>
+      <c r="T14" s="91"/>
+      <c r="U14" s="92"/>
+      <c r="V14" s="64"/>
+      <c r="W14" s="91"/>
+      <c r="X14" s="91"/>
+      <c r="Y14" s="91"/>
+      <c r="Z14" s="91"/>
+      <c r="AA14" s="91"/>
+      <c r="AB14" s="91"/>
+      <c r="AC14" s="91"/>
+      <c r="AD14" s="91"/>
+      <c r="AE14" s="91"/>
+      <c r="AF14" s="91"/>
+      <c r="AG14" s="91"/>
+      <c r="AH14" s="92"/>
+      <c r="AI14" s="64"/>
+      <c r="AJ14" s="64"/>
+      <c r="AK14" s="64"/>
+      <c r="AL14" s="64"/>
+      <c r="AM14" s="64"/>
+      <c r="AN14" s="64"/>
+      <c r="AO14" s="64"/>
+      <c r="AP14" s="64"/>
+      <c r="AQ14" s="64"/>
+      <c r="AR14" s="69"/>
+    </row>
+    <row r="15" spans="2:57" ht="14.25">
+      <c r="G15" s="68"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="63"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="76"/>
+      <c r="S15" s="97"/>
+      <c r="T15" s="102"/>
+      <c r="U15" s="103"/>
+      <c r="V15" s="98"/>
+      <c r="W15" s="102"/>
+      <c r="X15" s="102"/>
+      <c r="Y15" s="102"/>
+      <c r="Z15" s="102"/>
+      <c r="AA15" s="102"/>
+      <c r="AB15" s="102"/>
+      <c r="AC15" s="102"/>
+      <c r="AD15" s="102"/>
+      <c r="AE15" s="102"/>
+      <c r="AF15" s="102"/>
+      <c r="AG15" s="102"/>
+      <c r="AH15" s="103"/>
+      <c r="AI15" s="64"/>
+      <c r="AJ15" s="64"/>
+      <c r="AK15" s="64"/>
+      <c r="AL15" s="64"/>
+      <c r="AM15" s="64"/>
+      <c r="AN15" s="64"/>
+      <c r="AO15" s="64"/>
+      <c r="AP15" s="64"/>
+      <c r="AQ15" s="64"/>
+      <c r="AR15" s="69"/>
+    </row>
+    <row r="16" spans="2:57" ht="14.25">
+      <c r="G16" s="68"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="63"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="63"/>
+      <c r="R16" s="68"/>
+      <c r="S16" s="64"/>
+      <c r="T16" s="64"/>
+      <c r="U16" s="64"/>
+      <c r="V16" s="64"/>
+      <c r="W16" s="64"/>
+      <c r="X16" s="64"/>
+      <c r="Y16" s="64"/>
+      <c r="Z16" s="64"/>
+      <c r="AA16" s="64"/>
+      <c r="AB16" s="64"/>
+      <c r="AC16" s="64"/>
+      <c r="AD16" s="64"/>
+      <c r="AE16" s="64"/>
+      <c r="AF16" s="64"/>
+      <c r="AG16" s="64"/>
+      <c r="AH16" s="69"/>
+      <c r="AI16" s="64"/>
+      <c r="AJ16" s="64"/>
+      <c r="AK16" s="64"/>
+      <c r="AL16" s="64"/>
+      <c r="AM16" s="64"/>
+      <c r="AN16" s="64"/>
+      <c r="AO16" s="64"/>
+      <c r="AP16" s="64"/>
+      <c r="AQ16" s="64"/>
+      <c r="AR16" s="69"/>
+    </row>
+    <row r="17" spans="7:44" ht="14.25">
+      <c r="G17" s="68"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="63"/>
+      <c r="P17" s="63"/>
+      <c r="Q17" s="63"/>
+      <c r="R17" s="90"/>
+      <c r="S17" s="89"/>
+      <c r="T17" s="89"/>
+      <c r="U17" s="89"/>
+      <c r="V17" s="89"/>
+      <c r="W17" s="89"/>
+      <c r="X17" s="65"/>
+      <c r="Y17" s="66"/>
+      <c r="Z17" s="66"/>
+      <c r="AA17" s="66"/>
+      <c r="AB17" s="66"/>
+      <c r="AC17" s="66"/>
+      <c r="AD17" s="66"/>
+      <c r="AE17" s="66"/>
+      <c r="AF17" s="66"/>
+      <c r="AG17" s="66"/>
+      <c r="AH17" s="67"/>
+      <c r="AI17" s="64"/>
+      <c r="AJ17" s="64"/>
+      <c r="AK17" s="64"/>
+      <c r="AL17" s="64"/>
+      <c r="AM17" s="64"/>
+      <c r="AN17" s="64"/>
+      <c r="AO17" s="64"/>
+      <c r="AP17" s="64"/>
+      <c r="AQ17" s="64"/>
+      <c r="AR17" s="69"/>
+    </row>
+    <row r="18" spans="7:44" ht="14.25" customHeight="1">
+      <c r="G18" s="68"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="63"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="63"/>
+      <c r="R18" s="88" t="s">
+        <v>95</v>
+      </c>
+      <c r="S18" s="91"/>
+      <c r="T18" s="91"/>
+      <c r="U18" s="91"/>
+      <c r="V18" s="91"/>
+      <c r="W18" s="92"/>
+      <c r="X18" s="64"/>
+      <c r="Y18" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z18" s="64"/>
+      <c r="AA18" s="64"/>
+      <c r="AB18" s="84"/>
+      <c r="AC18" s="85"/>
+      <c r="AD18" s="85"/>
+      <c r="AE18" s="85"/>
+      <c r="AF18" s="85"/>
+      <c r="AG18" s="86"/>
+      <c r="AH18" s="69"/>
+      <c r="AI18" s="64"/>
+      <c r="AJ18" s="64"/>
+      <c r="AK18" s="64"/>
+      <c r="AL18" s="64"/>
+      <c r="AM18" s="64"/>
+      <c r="AN18" s="64"/>
+      <c r="AO18" s="64"/>
+      <c r="AP18" s="64"/>
+      <c r="AQ18" s="64"/>
+      <c r="AR18" s="69"/>
+    </row>
+    <row r="19" spans="7:44" ht="14.25" customHeight="1">
+      <c r="G19" s="68"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="63"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="63"/>
+      <c r="R19" s="88"/>
+      <c r="S19" s="91"/>
+      <c r="T19" s="91"/>
+      <c r="U19" s="91"/>
+      <c r="V19" s="91"/>
+      <c r="W19" s="92"/>
+      <c r="X19" s="64"/>
+      <c r="Y19" s="64"/>
+      <c r="Z19" s="64"/>
+      <c r="AA19" s="64"/>
+      <c r="AB19" s="64"/>
+      <c r="AC19" s="64"/>
+      <c r="AD19" s="64"/>
+      <c r="AE19" s="64"/>
+      <c r="AF19" s="64"/>
+      <c r="AG19" s="64"/>
+      <c r="AH19" s="69"/>
+      <c r="AI19" s="64"/>
+      <c r="AJ19" s="64"/>
+      <c r="AK19" s="64"/>
+      <c r="AL19" s="64"/>
+      <c r="AM19" s="64"/>
+      <c r="AN19" s="64"/>
+      <c r="AO19" s="64"/>
+      <c r="AP19" s="64"/>
+      <c r="AQ19" s="64"/>
+      <c r="AR19" s="69"/>
+    </row>
+    <row r="20" spans="7:44" ht="14.25" customHeight="1">
+      <c r="G20" s="68"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="63"/>
+      <c r="R20" s="88"/>
+      <c r="S20" s="91"/>
+      <c r="T20" s="91"/>
+      <c r="U20" s="91"/>
+      <c r="V20" s="91"/>
+      <c r="W20" s="92"/>
+      <c r="X20" s="64"/>
+      <c r="Y20" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z20" s="64"/>
+      <c r="AA20" s="64"/>
+      <c r="AB20" s="84"/>
+      <c r="AC20" s="85"/>
+      <c r="AD20" s="85"/>
+      <c r="AE20" s="85"/>
+      <c r="AF20" s="85"/>
+      <c r="AG20" s="86"/>
+      <c r="AH20" s="69"/>
+      <c r="AI20" s="64"/>
+      <c r="AJ20" s="64"/>
+      <c r="AK20" s="64"/>
+      <c r="AL20" s="64"/>
+      <c r="AM20" s="64"/>
+      <c r="AN20" s="64"/>
+      <c r="AO20" s="64"/>
+      <c r="AP20" s="64"/>
+      <c r="AQ20" s="64"/>
+      <c r="AR20" s="69"/>
+    </row>
+    <row r="21" spans="7:44" ht="14.25" customHeight="1">
+      <c r="G21" s="68"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="63"/>
+      <c r="P21" s="63"/>
+      <c r="Q21" s="63"/>
+      <c r="R21" s="88"/>
+      <c r="S21" s="91"/>
+      <c r="T21" s="91"/>
+      <c r="U21" s="91"/>
+      <c r="V21" s="91"/>
+      <c r="W21" s="92"/>
+      <c r="X21" s="64"/>
+      <c r="Y21" s="64"/>
+      <c r="Z21" s="64"/>
+      <c r="AA21" s="64"/>
+      <c r="AB21" s="64"/>
+      <c r="AC21" s="64"/>
+      <c r="AD21" s="64"/>
+      <c r="AE21" s="64"/>
+      <c r="AF21" s="64"/>
+      <c r="AG21" s="64"/>
+      <c r="AH21" s="69"/>
+      <c r="AI21" s="64"/>
+      <c r="AJ21" s="64"/>
+      <c r="AK21" s="64"/>
+      <c r="AL21" s="64"/>
+      <c r="AM21" s="64"/>
+      <c r="AN21" s="64"/>
+      <c r="AO21" s="64"/>
+      <c r="AP21" s="64"/>
+      <c r="AQ21" s="64"/>
+      <c r="AR21" s="69"/>
+    </row>
+    <row r="22" spans="7:44" ht="14.25">
+      <c r="G22" s="68"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="63"/>
+      <c r="N22" s="63"/>
+      <c r="O22" s="63"/>
+      <c r="P22" s="63"/>
+      <c r="Q22" s="63"/>
+      <c r="R22" s="90"/>
+      <c r="S22" s="89"/>
+      <c r="T22" s="89"/>
+      <c r="U22" s="89"/>
+      <c r="V22" s="89"/>
+      <c r="W22" s="89"/>
+      <c r="X22" s="68"/>
+      <c r="Y22" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z22" s="64"/>
+      <c r="AA22" s="64"/>
+      <c r="AB22" s="87" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC22" s="85"/>
+      <c r="AD22" s="85"/>
+      <c r="AE22" s="85"/>
+      <c r="AF22" s="86"/>
+      <c r="AG22" s="73" t="s">
+        <v>98</v>
+      </c>
+      <c r="AH22" s="69"/>
+      <c r="AI22" s="64"/>
+      <c r="AJ22" s="64"/>
+      <c r="AK22" s="64"/>
+      <c r="AL22" s="64"/>
+      <c r="AM22" s="64"/>
+      <c r="AN22" s="64"/>
+      <c r="AO22" s="64"/>
+      <c r="AP22" s="64"/>
+      <c r="AQ22" s="64"/>
+      <c r="AR22" s="69"/>
+    </row>
+    <row r="23" spans="7:44" ht="14.25">
+      <c r="G23" s="68"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="63"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="63"/>
+      <c r="Q23" s="63"/>
+      <c r="R23" s="81" t="s">
+        <v>99</v>
+      </c>
+      <c r="S23" s="82"/>
+      <c r="T23" s="82"/>
+      <c r="U23" s="82"/>
+      <c r="V23" s="82"/>
+      <c r="W23" s="83"/>
+      <c r="X23" s="68"/>
+      <c r="Y23" s="64"/>
+      <c r="Z23" s="64"/>
+      <c r="AA23" s="64"/>
+      <c r="AB23" s="64"/>
+      <c r="AC23" s="64"/>
+      <c r="AD23" s="64"/>
+      <c r="AE23" s="64"/>
+      <c r="AF23" s="64"/>
+      <c r="AG23" s="64"/>
+      <c r="AH23" s="69"/>
+      <c r="AI23" s="64"/>
+      <c r="AJ23" s="64"/>
+      <c r="AK23" s="64"/>
+      <c r="AL23" s="64"/>
+      <c r="AM23" s="64"/>
+      <c r="AN23" s="64"/>
+      <c r="AO23" s="64"/>
+      <c r="AP23" s="64"/>
+      <c r="AQ23" s="64"/>
+      <c r="AR23" s="69"/>
+    </row>
+    <row r="24" spans="7:44" ht="14.25">
+      <c r="G24" s="68"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="63"/>
+      <c r="N24" s="63"/>
+      <c r="O24" s="63"/>
+      <c r="P24" s="63"/>
+      <c r="Q24" s="63"/>
+      <c r="R24" s="95"/>
+      <c r="S24" s="94"/>
+      <c r="T24" s="94"/>
+      <c r="U24" s="94"/>
+      <c r="V24" s="94"/>
+      <c r="W24" s="94"/>
+      <c r="X24" s="68"/>
+      <c r="Y24" s="64"/>
+      <c r="Z24" s="64"/>
+      <c r="AA24" s="64"/>
+      <c r="AB24" s="64"/>
+      <c r="AC24" s="64"/>
+      <c r="AD24" s="64"/>
+      <c r="AE24" s="84" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF24" s="85"/>
+      <c r="AG24" s="86"/>
+      <c r="AH24" s="69"/>
+      <c r="AI24" s="64"/>
+      <c r="AJ24" s="64"/>
+      <c r="AK24" s="64"/>
+      <c r="AL24" s="64"/>
+      <c r="AM24" s="64"/>
+      <c r="AN24" s="64"/>
+      <c r="AO24" s="64"/>
+      <c r="AP24" s="64"/>
+      <c r="AQ24" s="64"/>
+      <c r="AR24" s="69"/>
+    </row>
+    <row r="25" spans="7:44" ht="14.25" customHeight="1">
+      <c r="G25" s="68"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="64"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="63"/>
+      <c r="P25" s="63"/>
+      <c r="Q25" s="63"/>
+      <c r="R25" s="88" t="s">
+        <v>100</v>
+      </c>
+      <c r="S25" s="91"/>
+      <c r="T25" s="91"/>
+      <c r="U25" s="91"/>
+      <c r="V25" s="91"/>
+      <c r="W25" s="91"/>
+      <c r="X25" s="96"/>
+      <c r="Y25" s="71"/>
+      <c r="Z25" s="71"/>
+      <c r="AA25" s="71"/>
+      <c r="AB25" s="71"/>
+      <c r="AC25" s="71"/>
+      <c r="AD25" s="71"/>
+      <c r="AE25" s="71"/>
+      <c r="AF25" s="71"/>
+      <c r="AG25" s="71"/>
+      <c r="AH25" s="72"/>
+      <c r="AI25" s="64"/>
+      <c r="AJ25" s="64"/>
+      <c r="AK25" s="64"/>
+      <c r="AL25" s="64"/>
+      <c r="AM25" s="64"/>
+      <c r="AN25" s="64"/>
+      <c r="AO25" s="64"/>
+      <c r="AP25" s="64"/>
+      <c r="AQ25" s="64"/>
+      <c r="AR25" s="69"/>
+    </row>
+    <row r="26" spans="7:44" ht="14.25" customHeight="1">
+      <c r="G26" s="68"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="64"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
+      <c r="O26" s="63"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="63"/>
+      <c r="R26" s="88"/>
+      <c r="S26" s="91"/>
+      <c r="T26" s="91"/>
+      <c r="U26" s="91"/>
+      <c r="V26" s="91"/>
+      <c r="W26" s="91"/>
+      <c r="X26" s="64"/>
+      <c r="Y26" s="64"/>
+      <c r="Z26" s="64"/>
+      <c r="AA26" s="64"/>
+      <c r="AB26" s="64"/>
+      <c r="AC26" s="64"/>
+      <c r="AD26" s="64"/>
+      <c r="AE26" s="64"/>
+      <c r="AF26" s="64"/>
+      <c r="AG26" s="64"/>
+      <c r="AH26" s="69"/>
+      <c r="AI26" s="64"/>
+      <c r="AJ26" s="64"/>
+      <c r="AK26" s="64"/>
+      <c r="AL26" s="64"/>
+      <c r="AM26" s="64"/>
+      <c r="AN26" s="64"/>
+      <c r="AO26" s="64"/>
+      <c r="AP26" s="64"/>
+      <c r="AQ26" s="64"/>
+      <c r="AR26" s="69"/>
+    </row>
+    <row r="27" spans="7:44" ht="14.25" customHeight="1">
+      <c r="G27" s="68"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="64"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="88"/>
+      <c r="S27" s="91"/>
+      <c r="T27" s="91"/>
+      <c r="U27" s="91"/>
+      <c r="V27" s="91"/>
+      <c r="W27" s="91"/>
+      <c r="X27" s="64"/>
+      <c r="Y27" s="64"/>
+      <c r="Z27" s="64"/>
+      <c r="AA27" s="64"/>
+      <c r="AB27" s="64"/>
+      <c r="AC27" s="64"/>
+      <c r="AD27" s="64"/>
+      <c r="AE27" s="64"/>
+      <c r="AF27" s="64"/>
+      <c r="AG27" s="64"/>
+      <c r="AH27" s="69"/>
+      <c r="AI27" s="64"/>
+      <c r="AJ27" s="64"/>
+      <c r="AK27" s="64"/>
+      <c r="AL27" s="64"/>
+      <c r="AM27" s="64"/>
+      <c r="AN27" s="64"/>
+      <c r="AO27" s="64"/>
+      <c r="AP27" s="64"/>
+      <c r="AQ27" s="64"/>
+      <c r="AR27" s="69"/>
+    </row>
+    <row r="28" spans="7:44" ht="14.25" customHeight="1">
+      <c r="G28" s="68"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="64"/>
+      <c r="J28" s="64"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="64"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="63"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="63"/>
+      <c r="Q28" s="63"/>
+      <c r="R28" s="93"/>
+      <c r="S28" s="99"/>
+      <c r="T28" s="99"/>
+      <c r="U28" s="99"/>
+      <c r="V28" s="99"/>
+      <c r="W28" s="99"/>
+      <c r="X28" s="71"/>
+      <c r="Y28" s="71"/>
+      <c r="Z28" s="71"/>
+      <c r="AA28" s="71"/>
+      <c r="AB28" s="71"/>
+      <c r="AC28" s="71"/>
+      <c r="AD28" s="71"/>
+      <c r="AE28" s="71"/>
+      <c r="AF28" s="71"/>
+      <c r="AG28" s="71"/>
+      <c r="AH28" s="72"/>
+      <c r="AI28" s="64"/>
+      <c r="AJ28" s="64"/>
+      <c r="AK28" s="64"/>
+      <c r="AL28" s="64"/>
+      <c r="AM28" s="64"/>
+      <c r="AN28" s="64"/>
+      <c r="AO28" s="64"/>
+      <c r="AP28" s="64"/>
+      <c r="AQ28" s="64"/>
+      <c r="AR28" s="69"/>
+    </row>
+    <row r="29" spans="7:44" ht="14.25">
+      <c r="G29" s="68"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
+      <c r="P29" s="63"/>
+      <c r="Q29" s="64"/>
+      <c r="R29" s="64"/>
+      <c r="S29" s="64"/>
+      <c r="T29" s="64"/>
+      <c r="U29" s="64"/>
+      <c r="V29" s="64"/>
+      <c r="W29" s="64"/>
+      <c r="X29" s="64"/>
+      <c r="Y29" s="64"/>
+      <c r="Z29" s="64"/>
+      <c r="AA29" s="64"/>
+      <c r="AB29" s="64"/>
+      <c r="AC29" s="64"/>
+      <c r="AD29" s="64"/>
+      <c r="AE29" s="64"/>
+      <c r="AF29" s="64"/>
+      <c r="AG29" s="64"/>
+      <c r="AH29" s="64"/>
+      <c r="AI29" s="64"/>
+      <c r="AJ29" s="64"/>
+      <c r="AK29" s="64"/>
+      <c r="AL29" s="64"/>
+      <c r="AM29" s="64"/>
+      <c r="AN29" s="64"/>
+      <c r="AO29" s="64"/>
+      <c r="AP29" s="64"/>
+      <c r="AQ29" s="64"/>
+      <c r="AR29" s="69"/>
+    </row>
+    <row r="30" spans="7:44" ht="14.25">
+      <c r="G30" s="68"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="64"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="64"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="64"/>
+      <c r="O30" s="64"/>
+      <c r="P30" s="64"/>
+      <c r="Q30" s="64"/>
+      <c r="R30" s="64"/>
+      <c r="S30" s="64"/>
+      <c r="T30" s="64"/>
+      <c r="U30" s="64"/>
+      <c r="V30" s="64"/>
+      <c r="W30" s="64"/>
+      <c r="X30" s="64"/>
+      <c r="Y30" s="64"/>
+      <c r="Z30" s="64"/>
+      <c r="AA30" s="64"/>
+      <c r="AB30" s="64"/>
+      <c r="AC30" s="64"/>
+      <c r="AD30" s="64"/>
+      <c r="AE30" s="64"/>
+      <c r="AF30" s="64"/>
+      <c r="AG30" s="64"/>
+      <c r="AH30" s="64"/>
+      <c r="AI30" s="64"/>
+      <c r="AJ30" s="64"/>
+      <c r="AK30" s="64"/>
+      <c r="AL30" s="64"/>
+      <c r="AM30" s="64"/>
+      <c r="AN30" s="64"/>
+      <c r="AO30" s="64"/>
+      <c r="AP30" s="64"/>
+      <c r="AQ30" s="64"/>
+      <c r="AR30" s="69"/>
+    </row>
+    <row r="31" spans="7:44" ht="14.25">
+      <c r="G31" s="68"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="64"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="64"/>
+      <c r="M31" s="64"/>
+      <c r="N31" s="64"/>
+      <c r="O31" s="64"/>
+      <c r="P31" s="64"/>
+      <c r="Q31" s="64"/>
+      <c r="R31" s="64"/>
+      <c r="S31" s="64"/>
+      <c r="T31" s="64"/>
+      <c r="U31" s="64"/>
+      <c r="V31" s="64"/>
+      <c r="W31" s="64"/>
+      <c r="X31" s="64"/>
+      <c r="Y31" s="64"/>
+      <c r="Z31" s="64"/>
+      <c r="AA31" s="64"/>
+      <c r="AB31" s="64"/>
+      <c r="AC31" s="64"/>
+      <c r="AD31" s="64"/>
+      <c r="AE31" s="64"/>
+      <c r="AF31" s="64"/>
+      <c r="AG31" s="64"/>
+      <c r="AH31" s="64"/>
+      <c r="AI31" s="64"/>
+      <c r="AJ31" s="64"/>
+      <c r="AK31" s="64"/>
+      <c r="AL31" s="64"/>
+      <c r="AM31" s="64"/>
+      <c r="AN31" s="64"/>
+      <c r="AO31" s="64"/>
+      <c r="AP31" s="64"/>
+      <c r="AQ31" s="64"/>
+      <c r="AR31" s="69"/>
+    </row>
+    <row r="32" spans="7:44" ht="14.25">
+      <c r="G32" s="68"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="64"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="64"/>
+      <c r="M32" s="64"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="64"/>
+      <c r="Q32" s="64"/>
+      <c r="R32" s="64"/>
+      <c r="S32" s="64"/>
+      <c r="T32" s="64"/>
+      <c r="U32" s="64"/>
+      <c r="V32" s="64"/>
+      <c r="W32" s="64"/>
+      <c r="X32" s="64"/>
+      <c r="Y32" s="64"/>
+      <c r="Z32" s="64"/>
+      <c r="AA32" s="64"/>
+      <c r="AB32" s="64"/>
+      <c r="AC32" s="64"/>
+      <c r="AD32" s="64"/>
+      <c r="AE32" s="64"/>
+      <c r="AF32" s="64"/>
+      <c r="AG32" s="64"/>
+      <c r="AH32" s="64"/>
+      <c r="AI32" s="64"/>
+      <c r="AJ32" s="64"/>
+      <c r="AK32" s="64"/>
+      <c r="AL32" s="64"/>
+      <c r="AM32" s="64"/>
+      <c r="AN32" s="64"/>
+      <c r="AO32" s="64"/>
+      <c r="AP32" s="64"/>
+      <c r="AQ32" s="64"/>
+      <c r="AR32" s="69"/>
+    </row>
+    <row r="33" spans="3:56" ht="14.25">
+      <c r="G33" s="68"/>
+      <c r="H33" s="64"/>
+      <c r="I33" s="64"/>
+      <c r="J33" s="64"/>
+      <c r="K33" s="64"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="64"/>
+      <c r="N33" s="64"/>
+      <c r="O33" s="64"/>
+      <c r="P33" s="64"/>
+      <c r="Q33" s="64"/>
+      <c r="R33" s="64"/>
+      <c r="S33" s="64"/>
+      <c r="T33" s="64"/>
+      <c r="U33" s="64"/>
+      <c r="V33" s="64"/>
+      <c r="W33" s="64"/>
+      <c r="X33" s="64"/>
+      <c r="Y33" s="64"/>
+      <c r="Z33" s="64"/>
+      <c r="AA33" s="64"/>
+      <c r="AB33" s="64"/>
+      <c r="AC33" s="64"/>
+      <c r="AD33" s="64"/>
+      <c r="AE33" s="64"/>
+      <c r="AF33" s="64"/>
+      <c r="AG33" s="64"/>
+      <c r="AH33" s="64"/>
+      <c r="AI33" s="64"/>
+      <c r="AJ33" s="64"/>
+      <c r="AK33" s="64"/>
+      <c r="AL33" s="64"/>
+      <c r="AM33" s="64"/>
+      <c r="AN33" s="64"/>
+      <c r="AO33" s="64"/>
+      <c r="AP33" s="64"/>
+      <c r="AQ33" s="64"/>
+      <c r="AR33" s="69"/>
+    </row>
+    <row r="34" spans="3:56" ht="14.25">
+      <c r="G34" s="68"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="64"/>
+      <c r="J34" s="64"/>
+      <c r="K34" s="64"/>
+      <c r="L34" s="64"/>
+      <c r="M34" s="64"/>
+      <c r="N34" s="64"/>
+      <c r="O34" s="64"/>
+      <c r="P34" s="64"/>
+      <c r="Q34" s="64"/>
+      <c r="R34" s="64"/>
+      <c r="S34" s="64"/>
+      <c r="T34" s="64"/>
+      <c r="U34" s="64"/>
+      <c r="V34" s="64"/>
+      <c r="W34" s="64"/>
+      <c r="X34" s="64"/>
+      <c r="Y34" s="64"/>
+      <c r="Z34" s="64"/>
+      <c r="AA34" s="64"/>
+      <c r="AB34" s="64"/>
+      <c r="AC34" s="64"/>
+      <c r="AD34" s="64"/>
+      <c r="AE34" s="64"/>
+      <c r="AF34" s="64"/>
+      <c r="AG34" s="64"/>
+      <c r="AH34" s="64"/>
+      <c r="AI34" s="64"/>
+      <c r="AJ34" s="64"/>
+      <c r="AK34" s="64"/>
+      <c r="AL34" s="64"/>
+      <c r="AM34" s="64"/>
+      <c r="AN34" s="64"/>
+      <c r="AO34" s="64"/>
+      <c r="AP34" s="64"/>
+      <c r="AQ34" s="64"/>
+      <c r="AR34" s="69"/>
+    </row>
+    <row r="35" spans="3:56" ht="14.25">
+      <c r="G35" s="70"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="71"/>
+      <c r="K35" s="71"/>
+      <c r="L35" s="71"/>
+      <c r="M35" s="71"/>
+      <c r="N35" s="71"/>
+      <c r="O35" s="71"/>
+      <c r="P35" s="71"/>
+      <c r="Q35" s="71"/>
+      <c r="R35" s="71"/>
+      <c r="S35" s="71"/>
+      <c r="T35" s="71"/>
+      <c r="U35" s="71"/>
+      <c r="V35" s="71"/>
+      <c r="W35" s="71"/>
+      <c r="X35" s="71"/>
+      <c r="Y35" s="71"/>
+      <c r="Z35" s="71"/>
+      <c r="AA35" s="71"/>
+      <c r="AB35" s="71"/>
+      <c r="AC35" s="71"/>
+      <c r="AD35" s="71"/>
+      <c r="AE35" s="71"/>
+      <c r="AF35" s="71"/>
+      <c r="AG35" s="71"/>
+      <c r="AH35" s="71"/>
+      <c r="AI35" s="71"/>
+      <c r="AJ35" s="71"/>
+      <c r="AK35" s="71"/>
+      <c r="AL35" s="71"/>
+      <c r="AM35" s="71"/>
+      <c r="AN35" s="71"/>
+      <c r="AO35" s="71"/>
+      <c r="AP35" s="71"/>
+      <c r="AQ35" s="71"/>
+      <c r="AR35" s="72"/>
+    </row>
+    <row r="39" spans="3:56">
+      <c r="C39" s="33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="3:56" ht="15">
+      <c r="C42" s="62" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="3:3">
-      <c r="C31" s="33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="3:56" ht="15">
-      <c r="C34" s="49" t="s">
+      <c r="D42" s="55"/>
+      <c r="E42" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="50"/>
-      <c r="E34" s="35" t="s">
+      <c r="F42" s="55"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="55"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="55"/>
+      <c r="M42" s="55"/>
+      <c r="N42" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="35"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="35"/>
-      <c r="L34" s="35"/>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35" t="s">
+      <c r="O42" s="55"/>
+      <c r="P42" s="55"/>
+      <c r="Q42" s="55"/>
+      <c r="R42" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="O34" s="35"/>
-      <c r="P34" s="35"/>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="35" t="s">
+      <c r="S42" s="55"/>
+      <c r="T42" s="55"/>
+      <c r="U42" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="S34" s="35"/>
-      <c r="T34" s="35"/>
-      <c r="U34" s="35" t="s">
+      <c r="V42" s="55"/>
+      <c r="W42" s="55"/>
+      <c r="X42" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="V34" s="35"/>
-      <c r="W34" s="35"/>
-      <c r="X34" s="35" t="s">
+      <c r="Y42" s="55"/>
+      <c r="Z42" s="55"/>
+      <c r="AA42" s="55"/>
+      <c r="AB42" s="55"/>
+      <c r="AC42" s="55"/>
+      <c r="AD42" s="55"/>
+      <c r="AE42" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="Y34" s="35"/>
-      <c r="Z34" s="35"/>
-      <c r="AA34" s="35"/>
-      <c r="AB34" s="35"/>
-      <c r="AC34" s="35"/>
-      <c r="AD34" s="35"/>
-      <c r="AE34" s="35" t="s">
+      <c r="AF42" s="55"/>
+      <c r="AG42" s="55"/>
+      <c r="AH42" s="55"/>
+      <c r="AI42" s="55"/>
+      <c r="AJ42" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="AF34" s="35"/>
-      <c r="AG34" s="35"/>
-      <c r="AH34" s="35"/>
-      <c r="AI34" s="35"/>
-      <c r="AJ34" s="35" t="s">
+      <c r="AK42" s="55"/>
+      <c r="AL42" s="55"/>
+      <c r="AM42" s="55"/>
+      <c r="AN42" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="AK34" s="35"/>
-      <c r="AL34" s="35"/>
-      <c r="AM34" s="35"/>
-      <c r="AN34" s="35" t="s">
+      <c r="AO42" s="55"/>
+      <c r="AP42" s="55"/>
+      <c r="AQ42" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="AO34" s="35"/>
-      <c r="AP34" s="35"/>
-      <c r="AQ34" s="35" t="s">
+      <c r="AR42" s="55"/>
+      <c r="AS42" s="55"/>
+      <c r="AT42" s="55"/>
+      <c r="AU42" s="55"/>
+      <c r="AV42" s="55"/>
+      <c r="AW42" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="AR34" s="35"/>
-      <c r="AS34" s="35"/>
-      <c r="AT34" s="35"/>
-      <c r="AU34" s="35"/>
-      <c r="AV34" s="35"/>
-      <c r="AW34" s="35" t="s">
+      <c r="AX42" s="55"/>
+      <c r="AY42" s="55"/>
+      <c r="AZ42" s="55"/>
+      <c r="BA42" s="55"/>
+      <c r="BB42" s="55"/>
+      <c r="BC42" s="55"/>
+      <c r="BD42" s="58"/>
+    </row>
+    <row r="43" spans="3:56">
+      <c r="C43" s="35">
+        <v>1</v>
+      </c>
+      <c r="D43" s="36"/>
+      <c r="E43" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="36"/>
+      <c r="L43" s="36"/>
+      <c r="M43" s="36"/>
+      <c r="N43" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="O43" s="36"/>
+      <c r="P43" s="36"/>
+      <c r="Q43" s="36"/>
+      <c r="R43" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="AX34" s="35"/>
-      <c r="AY34" s="35"/>
-      <c r="AZ34" s="35"/>
-      <c r="BA34" s="35"/>
-      <c r="BB34" s="35"/>
-      <c r="BC34" s="35"/>
-      <c r="BD34" s="45"/>
-    </row>
-    <row r="35" spans="3:56">
-      <c r="C35" s="36">
+      <c r="S43" s="36"/>
+      <c r="T43" s="36"/>
+      <c r="U43" s="35"/>
+      <c r="V43" s="36"/>
+      <c r="W43" s="36"/>
+      <c r="X43" s="35"/>
+      <c r="Y43" s="36"/>
+      <c r="Z43" s="36"/>
+      <c r="AA43" s="37">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="36"/>
+      <c r="AC43" s="36"/>
+      <c r="AD43" s="36"/>
+      <c r="AE43" s="35"/>
+      <c r="AF43" s="36"/>
+      <c r="AG43" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH43" s="36"/>
+      <c r="AI43" s="36"/>
+      <c r="AJ43" s="35"/>
+      <c r="AK43" s="36"/>
+      <c r="AL43" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM43" s="36"/>
+      <c r="AN43" s="35"/>
+      <c r="AO43" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP43" s="36"/>
+      <c r="AQ43" s="35"/>
+      <c r="AR43" s="36"/>
+      <c r="AS43" s="36"/>
+      <c r="AT43" s="43">
         <v>1</v>
       </c>
-      <c r="D35" s="37"/>
-      <c r="E35" s="36" t="s">
+      <c r="AU43" s="36"/>
+      <c r="AV43" s="36"/>
+      <c r="AW43" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
-      <c r="N35" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="O35" s="37"/>
-      <c r="P35" s="37"/>
-      <c r="Q35" s="37"/>
-      <c r="R35" s="36" t="s">
+      <c r="AX43" s="36"/>
+      <c r="AY43" s="36"/>
+      <c r="AZ43" s="36"/>
+      <c r="BA43" s="36"/>
+      <c r="BB43" s="36"/>
+      <c r="BC43" s="36"/>
+      <c r="BD43" s="38"/>
+    </row>
+    <row r="44" spans="3:56">
+      <c r="C44" s="35">
+        <v>2</v>
+      </c>
+      <c r="D44" s="40"/>
+      <c r="E44" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="40"/>
+      <c r="N44" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O44" s="40"/>
+      <c r="P44" s="40"/>
+      <c r="Q44" s="40"/>
+      <c r="R44" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="S44" s="40"/>
+      <c r="T44" s="40"/>
+      <c r="U44" s="39"/>
+      <c r="V44" s="40"/>
+      <c r="W44" s="40"/>
+      <c r="X44" s="39"/>
+      <c r="Y44" s="40"/>
+      <c r="Z44" s="40"/>
+      <c r="AA44" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="40"/>
+      <c r="AC44" s="40"/>
+      <c r="AD44" s="40"/>
+      <c r="AE44" s="39"/>
+      <c r="AF44" s="40"/>
+      <c r="AG44" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="S35" s="37"/>
-      <c r="T35" s="37"/>
-      <c r="U35" s="36"/>
-      <c r="V35" s="37"/>
-      <c r="W35" s="37"/>
-      <c r="X35" s="36"/>
-      <c r="Y35" s="37"/>
-      <c r="Z35" s="37"/>
-      <c r="AA35" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB35" s="37"/>
-      <c r="AC35" s="37"/>
-      <c r="AD35" s="37"/>
-      <c r="AE35" s="36"/>
-      <c r="AF35" s="37"/>
-      <c r="AG35" s="38" t="s">
+      <c r="AH44" s="40"/>
+      <c r="AI44" s="40"/>
+      <c r="AJ44" s="39"/>
+      <c r="AK44" s="40"/>
+      <c r="AL44" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM44" s="40"/>
+      <c r="AN44" s="39"/>
+      <c r="AO44" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP44" s="40"/>
+      <c r="AQ44" s="39"/>
+      <c r="AR44" s="40"/>
+      <c r="AS44" s="40"/>
+      <c r="AT44" s="43">
+        <v>1</v>
+      </c>
+      <c r="AU44" s="40"/>
+      <c r="AV44" s="40"/>
+      <c r="AW44" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="AX44" s="40"/>
+      <c r="AY44" s="40"/>
+      <c r="AZ44" s="40"/>
+      <c r="BA44" s="40"/>
+      <c r="BB44" s="40"/>
+      <c r="BC44" s="40"/>
+      <c r="BD44" s="42"/>
+    </row>
+    <row r="45" spans="3:56">
+      <c r="C45" s="35">
+        <v>3</v>
+      </c>
+      <c r="D45" s="40"/>
+      <c r="E45" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="40"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="40"/>
+      <c r="N45" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O45" s="40"/>
+      <c r="P45" s="40"/>
+      <c r="Q45" s="40"/>
+      <c r="R45" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="S45" s="40"/>
+      <c r="T45" s="40"/>
+      <c r="U45" s="39"/>
+      <c r="V45" s="40"/>
+      <c r="W45" s="40"/>
+      <c r="X45" s="39"/>
+      <c r="Y45" s="40"/>
+      <c r="Z45" s="40"/>
+      <c r="AA45" s="41">
+        <v>1</v>
+      </c>
+      <c r="AB45" s="40"/>
+      <c r="AC45" s="40"/>
+      <c r="AD45" s="40"/>
+      <c r="AE45" s="39"/>
+      <c r="AF45" s="40"/>
+      <c r="AG45" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH45" s="40"/>
+      <c r="AI45" s="40"/>
+      <c r="AJ45" s="39"/>
+      <c r="AK45" s="40"/>
+      <c r="AL45" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM45" s="40"/>
+      <c r="AN45" s="39"/>
+      <c r="AO45" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP45" s="40"/>
+      <c r="AQ45" s="39"/>
+      <c r="AR45" s="40"/>
+      <c r="AS45" s="40"/>
+      <c r="AT45" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU45" s="40"/>
+      <c r="AV45" s="40"/>
+      <c r="AW45" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX45" s="40"/>
+      <c r="AY45" s="40"/>
+      <c r="AZ45" s="40"/>
+      <c r="BA45" s="40"/>
+      <c r="BB45" s="40"/>
+      <c r="BC45" s="40"/>
+      <c r="BD45" s="42"/>
+    </row>
+    <row r="46" spans="3:56">
+      <c r="C46" s="35">
+        <v>4</v>
+      </c>
+      <c r="D46" s="40"/>
+      <c r="E46" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="40"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="40"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="40"/>
+      <c r="N46" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="O46" s="40"/>
+      <c r="P46" s="40"/>
+      <c r="Q46" s="40"/>
+      <c r="R46" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="S46" s="40"/>
+      <c r="T46" s="40"/>
+      <c r="U46" s="39"/>
+      <c r="V46" s="40"/>
+      <c r="W46" s="40"/>
+      <c r="X46" s="39"/>
+      <c r="Y46" s="40"/>
+      <c r="Z46" s="40"/>
+      <c r="AA46" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB46" s="40"/>
+      <c r="AC46" s="40"/>
+      <c r="AD46" s="40"/>
+      <c r="AE46" s="39"/>
+      <c r="AF46" s="40"/>
+      <c r="AG46" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH46" s="40"/>
+      <c r="AI46" s="40"/>
+      <c r="AJ46" s="39"/>
+      <c r="AK46" s="40"/>
+      <c r="AL46" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM46" s="40"/>
+      <c r="AN46" s="39"/>
+      <c r="AO46" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP46" s="40"/>
+      <c r="AQ46" s="39"/>
+      <c r="AR46" s="40"/>
+      <c r="AS46" s="40"/>
+      <c r="AT46" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU46" s="40"/>
+      <c r="AV46" s="40"/>
+      <c r="AW46" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="AX46" s="40"/>
+      <c r="AY46" s="40"/>
+      <c r="AZ46" s="40"/>
+      <c r="BA46" s="40"/>
+      <c r="BB46" s="40"/>
+      <c r="BC46" s="40"/>
+      <c r="BD46" s="42"/>
+    </row>
+    <row r="47" spans="3:56">
+      <c r="C47" s="35">
+        <v>5</v>
+      </c>
+      <c r="D47" s="40"/>
+      <c r="E47" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="40"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="40"/>
+      <c r="L47" s="40"/>
+      <c r="M47" s="40"/>
+      <c r="N47" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="AH35" s="37"/>
-      <c r="AI35" s="37"/>
-      <c r="AJ35" s="36"/>
-      <c r="AK35" s="37"/>
-      <c r="AL35" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM35" s="37"/>
-      <c r="AN35" s="36"/>
-      <c r="AO35" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP35" s="37"/>
-      <c r="AQ35" s="36"/>
-      <c r="AR35" s="37"/>
-      <c r="AS35" s="37"/>
-      <c r="AT35" s="44">
+      <c r="O47" s="40"/>
+      <c r="P47" s="40"/>
+      <c r="Q47" s="40"/>
+      <c r="R47" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="S47" s="40"/>
+      <c r="T47" s="40"/>
+      <c r="U47" s="39"/>
+      <c r="V47" s="40"/>
+      <c r="W47" s="40"/>
+      <c r="X47" s="39"/>
+      <c r="Y47" s="40"/>
+      <c r="Z47" s="40"/>
+      <c r="AA47" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB47" s="40"/>
+      <c r="AC47" s="40"/>
+      <c r="AD47" s="40"/>
+      <c r="AE47" s="39"/>
+      <c r="AF47" s="40"/>
+      <c r="AG47" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH47" s="40"/>
+      <c r="AI47" s="40"/>
+      <c r="AJ47" s="39"/>
+      <c r="AK47" s="40"/>
+      <c r="AL47" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM47" s="40"/>
+      <c r="AN47" s="39"/>
+      <c r="AO47" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP47" s="40"/>
+      <c r="AQ47" s="39"/>
+      <c r="AR47" s="40"/>
+      <c r="AS47" s="40"/>
+      <c r="AT47" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU47" s="40"/>
+      <c r="AV47" s="40"/>
+      <c r="AW47" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="AX47" s="40"/>
+      <c r="AY47" s="40"/>
+      <c r="AZ47" s="40"/>
+      <c r="BA47" s="40"/>
+      <c r="BB47" s="40"/>
+      <c r="BC47" s="40"/>
+      <c r="BD47" s="42"/>
+    </row>
+    <row r="48" spans="3:56">
+      <c r="C48" s="35">
+        <v>6</v>
+      </c>
+      <c r="D48" s="40"/>
+      <c r="E48" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="40"/>
+      <c r="J48" s="40"/>
+      <c r="K48" s="40"/>
+      <c r="L48" s="40"/>
+      <c r="M48" s="40"/>
+      <c r="N48" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="O48" s="40"/>
+      <c r="P48" s="40"/>
+      <c r="Q48" s="40"/>
+      <c r="R48" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="S48" s="40"/>
+      <c r="T48" s="40"/>
+      <c r="U48" s="39"/>
+      <c r="V48" s="40"/>
+      <c r="W48" s="40"/>
+      <c r="X48" s="39"/>
+      <c r="Y48" s="40"/>
+      <c r="Z48" s="40"/>
+      <c r="AA48" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB48" s="40"/>
+      <c r="AC48" s="40"/>
+      <c r="AD48" s="40"/>
+      <c r="AE48" s="39"/>
+      <c r="AF48" s="40"/>
+      <c r="AG48" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH48" s="40"/>
+      <c r="AI48" s="40"/>
+      <c r="AJ48" s="39"/>
+      <c r="AK48" s="40"/>
+      <c r="AL48" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM48" s="40"/>
+      <c r="AN48" s="39"/>
+      <c r="AO48" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP48" s="40"/>
+      <c r="AQ48" s="39"/>
+      <c r="AR48" s="40"/>
+      <c r="AS48" s="40"/>
+      <c r="AT48" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU48" s="40"/>
+      <c r="AV48" s="40"/>
+      <c r="AW48" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="AX48" s="40"/>
+      <c r="AY48" s="40"/>
+      <c r="AZ48" s="40"/>
+      <c r="BA48" s="40"/>
+      <c r="BB48" s="40"/>
+      <c r="BC48" s="40"/>
+      <c r="BD48" s="42"/>
+    </row>
+    <row r="52" spans="3:56">
+      <c r="C52" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="3:56">
+      <c r="C53" s="33"/>
+    </row>
+    <row r="54" spans="3:56" ht="15">
+      <c r="C54" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54" s="59"/>
+      <c r="E54" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="F54" s="59"/>
+      <c r="G54" s="59"/>
+      <c r="H54" s="59"/>
+      <c r="I54" s="59"/>
+      <c r="J54" s="59"/>
+      <c r="K54" s="59"/>
+      <c r="L54" s="59"/>
+      <c r="M54" s="59"/>
+      <c r="N54" s="59"/>
+      <c r="O54" s="59"/>
+      <c r="P54" s="59"/>
+      <c r="Q54" s="59"/>
+      <c r="R54" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="S54" s="59"/>
+      <c r="T54" s="59"/>
+      <c r="U54" s="59"/>
+      <c r="V54" s="59"/>
+      <c r="W54" s="59"/>
+      <c r="X54" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y54" s="59"/>
+      <c r="Z54" s="59"/>
+      <c r="AA54" s="59"/>
+      <c r="AB54" s="59"/>
+      <c r="AC54" s="59"/>
+      <c r="AD54" s="59"/>
+      <c r="AE54" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF54" s="59"/>
+      <c r="AG54" s="59"/>
+      <c r="AH54" s="59"/>
+      <c r="AI54" s="59"/>
+      <c r="AJ54" s="59"/>
+      <c r="AK54" s="59"/>
+      <c r="AL54" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM54" s="59"/>
+      <c r="AN54" s="59"/>
+      <c r="AO54" s="59"/>
+      <c r="AP54" s="59"/>
+      <c r="AQ54" s="59"/>
+      <c r="AR54" s="59"/>
+      <c r="AS54" s="59"/>
+      <c r="AT54" s="59"/>
+      <c r="AU54" s="59"/>
+      <c r="AV54" s="59"/>
+      <c r="AW54" s="59"/>
+      <c r="AX54" s="59"/>
+      <c r="AY54" s="59"/>
+      <c r="AZ54" s="59"/>
+      <c r="BA54" s="59"/>
+      <c r="BB54" s="59"/>
+      <c r="BC54" s="59"/>
+      <c r="BD54" s="60"/>
+    </row>
+    <row r="55" spans="3:56">
+      <c r="C55" s="46">
         <v>1</v>
       </c>
-      <c r="AU35" s="37"/>
-      <c r="AV35" s="37"/>
-      <c r="AW35" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX35" s="37"/>
-      <c r="AY35" s="37"/>
-      <c r="AZ35" s="37"/>
-      <c r="BA35" s="37"/>
-      <c r="BB35" s="37"/>
-      <c r="BC35" s="37"/>
-      <c r="BD35" s="39"/>
-    </row>
-    <row r="36" spans="3:56">
-      <c r="C36" s="36">
+      <c r="D55" s="38"/>
+      <c r="E55" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="F55" s="36"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="36"/>
+      <c r="J55" s="36"/>
+      <c r="K55" s="36"/>
+      <c r="L55" s="36"/>
+      <c r="M55" s="36"/>
+      <c r="N55" s="36"/>
+      <c r="O55" s="36"/>
+      <c r="P55" s="36"/>
+      <c r="Q55" s="38"/>
+      <c r="R55" s="36"/>
+      <c r="S55" s="36"/>
+      <c r="T55" s="36"/>
+      <c r="U55" s="36"/>
+      <c r="V55" s="36"/>
+      <c r="W55" s="38"/>
+      <c r="X55" s="36"/>
+      <c r="Y55" s="36"/>
+      <c r="Z55" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA55" s="36"/>
+      <c r="AB55" s="36"/>
+      <c r="AC55" s="36"/>
+      <c r="AD55" s="38"/>
+      <c r="AF55" s="36"/>
+      <c r="AG55" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH55" s="36"/>
+      <c r="AI55" s="36"/>
+      <c r="AJ55" s="36"/>
+      <c r="AK55" s="38"/>
+      <c r="AL55" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM55" s="36"/>
+      <c r="AN55" s="36"/>
+      <c r="AO55" s="36"/>
+      <c r="AP55" s="36"/>
+      <c r="AQ55" s="36"/>
+      <c r="AR55" s="36"/>
+      <c r="AS55" s="36"/>
+      <c r="AT55" s="36"/>
+      <c r="AU55" s="36"/>
+      <c r="AV55" s="36"/>
+      <c r="AW55" s="36"/>
+      <c r="AX55" s="36"/>
+      <c r="AY55" s="36"/>
+      <c r="AZ55" s="36"/>
+      <c r="BA55" s="36"/>
+      <c r="BB55" s="36"/>
+      <c r="BC55" s="36"/>
+      <c r="BD55" s="38"/>
+    </row>
+    <row r="56" spans="3:56">
+      <c r="C56" s="47">
         <v>2</v>
       </c>
-      <c r="D36" s="41"/>
-      <c r="E36" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="41"/>
-      <c r="L36" s="41"/>
-      <c r="M36" s="41"/>
-      <c r="N36" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="O36" s="41"/>
-      <c r="P36" s="41"/>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="S36" s="41"/>
-      <c r="T36" s="41"/>
-      <c r="U36" s="40"/>
-      <c r="V36" s="41"/>
-      <c r="W36" s="41"/>
-      <c r="X36" s="40"/>
-      <c r="Y36" s="41"/>
-      <c r="Z36" s="41"/>
-      <c r="AA36" s="42">
-        <v>0</v>
-      </c>
-      <c r="AB36" s="41"/>
-      <c r="AC36" s="41"/>
-      <c r="AD36" s="41"/>
-      <c r="AE36" s="40"/>
-      <c r="AF36" s="41"/>
-      <c r="AG36" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH36" s="41"/>
-      <c r="AI36" s="41"/>
-      <c r="AJ36" s="40"/>
-      <c r="AK36" s="41"/>
-      <c r="AL36" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM36" s="41"/>
-      <c r="AN36" s="40"/>
-      <c r="AO36" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP36" s="41"/>
-      <c r="AQ36" s="40"/>
-      <c r="AR36" s="41"/>
-      <c r="AS36" s="41"/>
-      <c r="AT36" s="44">
+      <c r="D56" s="42"/>
+      <c r="E56" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="40"/>
+      <c r="J56" s="40"/>
+      <c r="K56" s="40"/>
+      <c r="L56" s="40"/>
+      <c r="M56" s="40"/>
+      <c r="N56" s="40"/>
+      <c r="O56" s="40"/>
+      <c r="P56" s="40"/>
+      <c r="Q56" s="42"/>
+      <c r="R56" s="40"/>
+      <c r="S56" s="40"/>
+      <c r="T56" s="40"/>
+      <c r="U56" s="40"/>
+      <c r="V56" s="40"/>
+      <c r="W56" s="42"/>
+      <c r="X56" s="40"/>
+      <c r="Y56" s="40"/>
+      <c r="Z56" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA56" s="40"/>
+      <c r="AB56" s="40"/>
+      <c r="AC56" s="40"/>
+      <c r="AD56" s="42"/>
+      <c r="AE56" s="40"/>
+      <c r="AF56" s="40"/>
+      <c r="AG56" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH56" s="40"/>
+      <c r="AI56" s="40"/>
+      <c r="AJ56" s="40"/>
+      <c r="AK56" s="42"/>
+      <c r="AL56" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM56" s="40"/>
+      <c r="AN56" s="40"/>
+      <c r="AO56" s="40"/>
+      <c r="AP56" s="40"/>
+      <c r="AQ56" s="40"/>
+      <c r="AR56" s="40"/>
+      <c r="AS56" s="40"/>
+      <c r="AT56" s="40"/>
+      <c r="AU56" s="40"/>
+      <c r="AV56" s="40"/>
+      <c r="AW56" s="40"/>
+      <c r="AX56" s="40"/>
+      <c r="AY56" s="40"/>
+      <c r="AZ56" s="40"/>
+      <c r="BA56" s="40"/>
+      <c r="BB56" s="40"/>
+      <c r="BC56" s="40"/>
+      <c r="BD56" s="42"/>
+    </row>
+    <row r="57" spans="3:56">
+      <c r="C57" s="47">
+        <v>3</v>
+      </c>
+      <c r="D57" s="42"/>
+      <c r="E57" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="F57" s="40"/>
+      <c r="G57" s="40"/>
+      <c r="H57" s="40"/>
+      <c r="I57" s="40"/>
+      <c r="J57" s="40"/>
+      <c r="K57" s="40"/>
+      <c r="L57" s="40"/>
+      <c r="M57" s="40"/>
+      <c r="N57" s="40"/>
+      <c r="O57" s="40"/>
+      <c r="P57" s="40"/>
+      <c r="Q57" s="42"/>
+      <c r="R57" s="40"/>
+      <c r="S57" s="40"/>
+      <c r="T57" s="40"/>
+      <c r="U57" s="40"/>
+      <c r="V57" s="40"/>
+      <c r="W57" s="42"/>
+      <c r="X57" s="40"/>
+      <c r="Y57" s="40"/>
+      <c r="Z57" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA57" s="40"/>
+      <c r="AB57" s="40"/>
+      <c r="AC57" s="40"/>
+      <c r="AD57" s="42"/>
+      <c r="AE57" s="40"/>
+      <c r="AF57" s="40"/>
+      <c r="AG57" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH57" s="40"/>
+      <c r="AI57" s="40"/>
+      <c r="AJ57" s="40"/>
+      <c r="AK57" s="42"/>
+      <c r="AL57" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM57" s="40"/>
+      <c r="AN57" s="40"/>
+      <c r="AO57" s="40"/>
+      <c r="AP57" s="40"/>
+      <c r="AQ57" s="40"/>
+      <c r="AR57" s="40"/>
+      <c r="AS57" s="40"/>
+      <c r="AT57" s="40"/>
+      <c r="AU57" s="40"/>
+      <c r="AV57" s="40"/>
+      <c r="AW57" s="40"/>
+      <c r="AX57" s="40"/>
+      <c r="AY57" s="40"/>
+      <c r="AZ57" s="40"/>
+      <c r="BA57" s="40"/>
+      <c r="BB57" s="40"/>
+      <c r="BC57" s="40"/>
+      <c r="BD57" s="42"/>
+    </row>
+    <row r="58" spans="3:56">
+      <c r="C58" s="48">
+        <v>4</v>
+      </c>
+      <c r="D58" s="49"/>
+      <c r="E58" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="F58" s="50"/>
+      <c r="G58" s="50"/>
+      <c r="H58" s="50"/>
+      <c r="I58" s="50"/>
+      <c r="J58" s="50"/>
+      <c r="K58" s="50"/>
+      <c r="L58" s="50"/>
+      <c r="M58" s="50"/>
+      <c r="N58" s="50"/>
+      <c r="O58" s="50"/>
+      <c r="P58" s="50"/>
+      <c r="Q58" s="49"/>
+      <c r="R58" s="50"/>
+      <c r="S58" s="50"/>
+      <c r="T58" s="50"/>
+      <c r="U58" s="50"/>
+      <c r="V58" s="50"/>
+      <c r="W58" s="49"/>
+      <c r="X58" s="50"/>
+      <c r="Y58" s="50"/>
+      <c r="Z58" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA58" s="50"/>
+      <c r="AB58" s="50"/>
+      <c r="AC58" s="50"/>
+      <c r="AD58" s="49"/>
+      <c r="AE58" s="50"/>
+      <c r="AF58" s="50"/>
+      <c r="AG58" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH58" s="50"/>
+      <c r="AI58" s="50"/>
+      <c r="AJ58" s="50"/>
+      <c r="AK58" s="49"/>
+      <c r="AL58" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM58" s="50"/>
+      <c r="AN58" s="50"/>
+      <c r="AO58" s="50"/>
+      <c r="AP58" s="50"/>
+      <c r="AQ58" s="50"/>
+      <c r="AR58" s="50"/>
+      <c r="AS58" s="50"/>
+      <c r="AT58" s="50"/>
+      <c r="AU58" s="50"/>
+      <c r="AV58" s="50"/>
+      <c r="AW58" s="50"/>
+      <c r="AX58" s="50"/>
+      <c r="AY58" s="50"/>
+      <c r="AZ58" s="50"/>
+      <c r="BA58" s="50"/>
+      <c r="BB58" s="50"/>
+      <c r="BC58" s="50"/>
+      <c r="BD58" s="49"/>
+    </row>
+    <row r="60" spans="3:56">
+      <c r="C60" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="62" spans="3:56" ht="15">
+      <c r="C62" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="D62" s="59"/>
+      <c r="E62" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="F62" s="59"/>
+      <c r="G62" s="59"/>
+      <c r="H62" s="59"/>
+      <c r="I62" s="59"/>
+      <c r="J62" s="59"/>
+      <c r="K62" s="59"/>
+      <c r="L62" s="59"/>
+      <c r="M62" s="59"/>
+      <c r="N62" s="59"/>
+      <c r="O62" s="59"/>
+      <c r="P62" s="59"/>
+      <c r="Q62" s="59"/>
+      <c r="R62" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="S62" s="59"/>
+      <c r="T62" s="59"/>
+      <c r="U62" s="59"/>
+      <c r="V62" s="59"/>
+      <c r="W62" s="59"/>
+      <c r="X62" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y62" s="59"/>
+      <c r="Z62" s="59"/>
+      <c r="AA62" s="59"/>
+      <c r="AB62" s="59"/>
+      <c r="AC62" s="59"/>
+      <c r="AD62" s="59"/>
+      <c r="AE62" s="59"/>
+      <c r="AF62" s="59"/>
+      <c r="AG62" s="59"/>
+      <c r="AH62" s="59"/>
+      <c r="AI62" s="59"/>
+      <c r="AJ62" s="59"/>
+      <c r="AK62" s="59"/>
+      <c r="AL62" s="59"/>
+      <c r="AM62" s="59"/>
+      <c r="AN62" s="59"/>
+      <c r="AO62" s="59"/>
+      <c r="AP62" s="59"/>
+      <c r="AQ62" s="59"/>
+      <c r="AR62" s="59"/>
+      <c r="AS62" s="59"/>
+      <c r="AT62" s="59"/>
+      <c r="AU62" s="59"/>
+      <c r="AV62" s="59"/>
+      <c r="AW62" s="59"/>
+      <c r="AX62" s="59"/>
+      <c r="AY62" s="59"/>
+      <c r="AZ62" s="59"/>
+      <c r="BA62" s="59"/>
+      <c r="BB62" s="59"/>
+      <c r="BC62" s="59"/>
+      <c r="BD62" s="60"/>
+    </row>
+    <row r="63" spans="3:56">
+      <c r="C63" s="35">
         <v>1</v>
       </c>
-      <c r="AU36" s="41"/>
-      <c r="AV36" s="41"/>
-      <c r="AW36" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="AX36" s="41"/>
-      <c r="AY36" s="41"/>
-      <c r="AZ36" s="41"/>
-      <c r="BA36" s="41"/>
-      <c r="BB36" s="41"/>
-      <c r="BC36" s="41"/>
-      <c r="BD36" s="43"/>
-    </row>
-    <row r="37" spans="3:56">
-      <c r="C37" s="36">
-        <v>3</v>
-      </c>
-      <c r="D37" s="41"/>
-      <c r="E37" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="41"/>
-      <c r="L37" s="41"/>
-      <c r="M37" s="41"/>
-      <c r="N37" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="O37" s="41"/>
-      <c r="P37" s="41"/>
-      <c r="Q37" s="41"/>
-      <c r="R37" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="S37" s="41"/>
-      <c r="T37" s="41"/>
-      <c r="U37" s="40"/>
-      <c r="V37" s="41"/>
-      <c r="W37" s="41"/>
-      <c r="X37" s="40"/>
-      <c r="Y37" s="41"/>
-      <c r="Z37" s="41"/>
-      <c r="AA37" s="42">
-        <v>1</v>
-      </c>
-      <c r="AB37" s="41"/>
-      <c r="AC37" s="41"/>
-      <c r="AD37" s="41"/>
-      <c r="AE37" s="40"/>
-      <c r="AF37" s="41"/>
-      <c r="AG37" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH37" s="41"/>
-      <c r="AI37" s="41"/>
-      <c r="AJ37" s="40"/>
-      <c r="AK37" s="41"/>
-      <c r="AL37" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM37" s="41"/>
-      <c r="AN37" s="40"/>
-      <c r="AO37" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP37" s="41"/>
-      <c r="AQ37" s="40"/>
-      <c r="AR37" s="41"/>
-      <c r="AS37" s="41"/>
-      <c r="AT37" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AU37" s="41"/>
-      <c r="AV37" s="41"/>
-      <c r="AW37" s="40" t="s">
+      <c r="D63" s="38"/>
+      <c r="E63" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="F63" s="36"/>
+      <c r="G63" s="36"/>
+      <c r="H63" s="36"/>
+      <c r="I63" s="36"/>
+      <c r="J63" s="36"/>
+      <c r="K63" s="36"/>
+      <c r="L63" s="36"/>
+      <c r="M63" s="36"/>
+      <c r="N63" s="36"/>
+      <c r="O63" s="36"/>
+      <c r="P63" s="36"/>
+      <c r="Q63" s="38"/>
+      <c r="R63" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="S63" s="36"/>
+      <c r="T63" s="36"/>
+      <c r="U63" s="36"/>
+      <c r="V63" s="36"/>
+      <c r="W63" s="38"/>
+      <c r="X63" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y63" s="36"/>
+      <c r="Z63" s="36"/>
+      <c r="AA63" s="36"/>
+      <c r="AB63" s="36"/>
+      <c r="AC63" s="36"/>
+      <c r="AD63" s="36"/>
+      <c r="AE63" s="36"/>
+      <c r="AF63" s="36"/>
+      <c r="AG63" s="36"/>
+      <c r="AH63" s="36"/>
+      <c r="AI63" s="36"/>
+      <c r="AJ63" s="36"/>
+      <c r="AK63" s="36"/>
+      <c r="AL63" s="36"/>
+      <c r="AM63" s="36"/>
+      <c r="AN63" s="36"/>
+      <c r="AO63" s="36"/>
+      <c r="AP63" s="36"/>
+      <c r="AQ63" s="36"/>
+      <c r="AR63" s="36"/>
+      <c r="AS63" s="36"/>
+      <c r="AT63" s="36"/>
+      <c r="AU63" s="36"/>
+      <c r="AV63" s="36"/>
+      <c r="AW63" s="36"/>
+      <c r="AX63" s="36"/>
+      <c r="AY63" s="36"/>
+      <c r="AZ63" s="36"/>
+      <c r="BA63" s="36"/>
+      <c r="BB63" s="36"/>
+      <c r="BC63" s="36"/>
+      <c r="BD63" s="38"/>
+    </row>
+    <row r="64" spans="3:56">
+      <c r="C64" s="39">
+        <v>2</v>
+      </c>
+      <c r="D64" s="42"/>
+      <c r="E64" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="AX37" s="41"/>
-      <c r="AY37" s="41"/>
-      <c r="AZ37" s="41"/>
-      <c r="BA37" s="41"/>
-      <c r="BB37" s="41"/>
-      <c r="BC37" s="41"/>
-      <c r="BD37" s="43"/>
-    </row>
-    <row r="38" spans="3:56">
-      <c r="C38" s="36">
-        <v>4</v>
-      </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="41"/>
-      <c r="L38" s="41"/>
-      <c r="M38" s="41"/>
-      <c r="N38" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="O38" s="41"/>
-      <c r="P38" s="41"/>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="S38" s="41"/>
-      <c r="T38" s="41"/>
-      <c r="U38" s="40"/>
-      <c r="V38" s="41"/>
-      <c r="W38" s="41"/>
-      <c r="X38" s="40"/>
-      <c r="Y38" s="41"/>
-      <c r="Z38" s="41"/>
-      <c r="AA38" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB38" s="41"/>
-      <c r="AC38" s="41"/>
-      <c r="AD38" s="41"/>
-      <c r="AE38" s="40"/>
-      <c r="AF38" s="41"/>
-      <c r="AG38" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH38" s="41"/>
-      <c r="AI38" s="41"/>
-      <c r="AJ38" s="40"/>
-      <c r="AK38" s="41"/>
-      <c r="AL38" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM38" s="41"/>
-      <c r="AN38" s="40"/>
-      <c r="AO38" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP38" s="41"/>
-      <c r="AQ38" s="40"/>
-      <c r="AR38" s="41"/>
-      <c r="AS38" s="41"/>
-      <c r="AT38" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AU38" s="41"/>
-      <c r="AV38" s="41"/>
-      <c r="AW38" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX38" s="41"/>
-      <c r="AY38" s="41"/>
-      <c r="AZ38" s="41"/>
-      <c r="BA38" s="41"/>
-      <c r="BB38" s="41"/>
-      <c r="BC38" s="41"/>
-      <c r="BD38" s="43"/>
-    </row>
-    <row r="39" spans="3:56">
-      <c r="C39" s="36">
-        <v>5</v>
-      </c>
-      <c r="D39" s="41"/>
-      <c r="E39" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="41"/>
-      <c r="L39" s="41"/>
-      <c r="M39" s="41"/>
-      <c r="N39" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="O39" s="41"/>
-      <c r="P39" s="41"/>
-      <c r="Q39" s="41"/>
-      <c r="R39" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="S39" s="41"/>
-      <c r="T39" s="41"/>
-      <c r="U39" s="40"/>
-      <c r="V39" s="41"/>
-      <c r="W39" s="41"/>
-      <c r="X39" s="40"/>
-      <c r="Y39" s="41"/>
-      <c r="Z39" s="41"/>
-      <c r="AA39" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB39" s="41"/>
-      <c r="AC39" s="41"/>
-      <c r="AD39" s="41"/>
-      <c r="AE39" s="40"/>
-      <c r="AF39" s="41"/>
-      <c r="AG39" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH39" s="41"/>
-      <c r="AI39" s="41"/>
-      <c r="AJ39" s="40"/>
-      <c r="AK39" s="41"/>
-      <c r="AL39" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM39" s="41"/>
-      <c r="AN39" s="40"/>
-      <c r="AO39" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP39" s="41"/>
-      <c r="AQ39" s="40"/>
-      <c r="AR39" s="41"/>
-      <c r="AS39" s="41"/>
-      <c r="AT39" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AU39" s="41"/>
-      <c r="AV39" s="41"/>
-      <c r="AW39" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="AX39" s="41"/>
-      <c r="AY39" s="41"/>
-      <c r="AZ39" s="41"/>
-      <c r="BA39" s="41"/>
-      <c r="BB39" s="41"/>
-      <c r="BC39" s="41"/>
-      <c r="BD39" s="43"/>
-    </row>
-    <row r="40" spans="3:56">
-      <c r="C40" s="36">
-        <v>6</v>
-      </c>
-      <c r="D40" s="41"/>
-      <c r="E40" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="F40" s="41"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41"/>
-      <c r="J40" s="41"/>
-      <c r="K40" s="41"/>
-      <c r="L40" s="41"/>
-      <c r="M40" s="41"/>
-      <c r="N40" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="O40" s="41"/>
-      <c r="P40" s="41"/>
-      <c r="Q40" s="41"/>
-      <c r="R40" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="S40" s="41"/>
-      <c r="T40" s="41"/>
-      <c r="U40" s="40"/>
-      <c r="V40" s="41"/>
-      <c r="W40" s="41"/>
-      <c r="X40" s="40"/>
-      <c r="Y40" s="41"/>
-      <c r="Z40" s="41"/>
-      <c r="AA40" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB40" s="41"/>
-      <c r="AC40" s="41"/>
-      <c r="AD40" s="41"/>
-      <c r="AE40" s="40"/>
-      <c r="AF40" s="41"/>
-      <c r="AG40" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH40" s="41"/>
-      <c r="AI40" s="41"/>
-      <c r="AJ40" s="40"/>
-      <c r="AK40" s="41"/>
-      <c r="AL40" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM40" s="41"/>
-      <c r="AN40" s="40"/>
-      <c r="AO40" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP40" s="41"/>
-      <c r="AQ40" s="40"/>
-      <c r="AR40" s="41"/>
-      <c r="AS40" s="41"/>
-      <c r="AT40" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="AU40" s="41"/>
-      <c r="AV40" s="41"/>
-      <c r="AW40" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="AX40" s="41"/>
-      <c r="AY40" s="41"/>
-      <c r="AZ40" s="41"/>
-      <c r="BA40" s="41"/>
-      <c r="BB40" s="41"/>
-      <c r="BC40" s="41"/>
-      <c r="BD40" s="43"/>
-    </row>
-    <row r="44" spans="3:56">
-      <c r="C44" s="33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3">
-      <c r="C54" s="33" t="s">
-        <v>34</v>
-      </c>
+      <c r="F64" s="40"/>
+      <c r="G64" s="40"/>
+      <c r="H64" s="40"/>
+      <c r="I64" s="40"/>
+      <c r="J64" s="40"/>
+      <c r="K64" s="40"/>
+      <c r="L64" s="40"/>
+      <c r="M64" s="40"/>
+      <c r="N64" s="40"/>
+      <c r="O64" s="40"/>
+      <c r="P64" s="40"/>
+      <c r="Q64" s="42"/>
+      <c r="R64" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="S64" s="40"/>
+      <c r="T64" s="40"/>
+      <c r="U64" s="40"/>
+      <c r="V64" s="40"/>
+      <c r="W64" s="42"/>
+      <c r="X64" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y64" s="40"/>
+      <c r="Z64" s="40"/>
+      <c r="AA64" s="40"/>
+      <c r="AB64" s="40"/>
+      <c r="AC64" s="40"/>
+      <c r="AD64" s="40"/>
+      <c r="AE64" s="40"/>
+      <c r="AF64" s="40"/>
+      <c r="AG64" s="40"/>
+      <c r="AH64" s="40"/>
+      <c r="AI64" s="40"/>
+      <c r="AJ64" s="40"/>
+      <c r="AK64" s="40"/>
+      <c r="AL64" s="40"/>
+      <c r="AM64" s="40"/>
+      <c r="AN64" s="40"/>
+      <c r="AO64" s="40"/>
+      <c r="AP64" s="40"/>
+      <c r="AQ64" s="40"/>
+      <c r="AR64" s="40"/>
+      <c r="AS64" s="40"/>
+      <c r="AT64" s="40"/>
+      <c r="AU64" s="40"/>
+      <c r="AV64" s="40"/>
+      <c r="AW64" s="40"/>
+      <c r="AX64" s="40"/>
+      <c r="AY64" s="40"/>
+      <c r="AZ64" s="40"/>
+      <c r="BA64" s="40"/>
+      <c r="BB64" s="40"/>
+      <c r="BC64" s="40"/>
+      <c r="BD64" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="45">
+    <mergeCell ref="AN42:AP42"/>
+    <mergeCell ref="R11:Z12"/>
+    <mergeCell ref="R23:W23"/>
+    <mergeCell ref="T13:U15"/>
+    <mergeCell ref="W13:AH15"/>
+    <mergeCell ref="AE24:AG24"/>
+    <mergeCell ref="AB18:AG18"/>
+    <mergeCell ref="AB20:AG20"/>
+    <mergeCell ref="AB22:AF22"/>
+    <mergeCell ref="R18:W21"/>
+    <mergeCell ref="R25:W28"/>
+    <mergeCell ref="AQ42:AV42"/>
+    <mergeCell ref="AW42:BD42"/>
+    <mergeCell ref="AL54:BD54"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:Q62"/>
+    <mergeCell ref="R62:W62"/>
+    <mergeCell ref="X62:BD62"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:Q54"/>
+    <mergeCell ref="R54:W54"/>
+    <mergeCell ref="X54:AD54"/>
+    <mergeCell ref="AE54:AK54"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:M42"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:AP3"/>
+    <mergeCell ref="AT4:AW4"/>
+    <mergeCell ref="AT5:AW5"/>
+    <mergeCell ref="F4:N4"/>
+    <mergeCell ref="F5:N5"/>
+    <mergeCell ref="AQ2:AW2"/>
+    <mergeCell ref="U42:W42"/>
+    <mergeCell ref="X42:AD42"/>
+    <mergeCell ref="AE42:AI42"/>
+    <mergeCell ref="AJ42:AM42"/>
     <mergeCell ref="AX2:BE2"/>
     <mergeCell ref="BB4:BE4"/>
     <mergeCell ref="BB5:BE5"/>
@@ -2542,19 +4780,12 @@
     <mergeCell ref="U5:AP5"/>
     <mergeCell ref="AQ3:AW3"/>
     <mergeCell ref="AX3:BE3"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="E2:AP3"/>
-    <mergeCell ref="AT4:AW4"/>
-    <mergeCell ref="AT5:AW5"/>
-    <mergeCell ref="F4:N4"/>
-    <mergeCell ref="F5:N5"/>
-    <mergeCell ref="AQ2:AW2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="98" orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="28" min="1" max="64" man="1"/>
+    <brk id="28" min="1" max="87" man="1"/>
   </colBreaks>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>